<commit_message>
adding polyAisolation method, media info, temperature info
</commit_message>
<xml_diff>
--- a/s1cDNASample/s1cDNASample_1272.xlsx
+++ b/s1cDNASample/s1cDNASample_1272.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/s1cDNASample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45FC334-9D0C-AB46-BA94-0E78902A8BF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A64181-672B-8E44-B9E5-A9480416D8C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="15680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="13">
   <si>
     <t>rnaDate</t>
   </si>
@@ -59,12 +59,18 @@
   <si>
     <t>S.GISH</t>
   </si>
+  <si>
+    <t>polyAIsolationProtocol</t>
+  </si>
+  <si>
+    <t>catcher</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -79,6 +85,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,11 +128,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,18 +448,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" activeCellId="1" sqref="B3:B29 E2:E29"/>
+      <selection activeCell="G3" sqref="G3:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="1026" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,11 +485,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -489,10 +512,13 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -512,10 +538,13 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -535,10 +564,13 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -558,10 +590,13 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -581,10 +616,13 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -604,10 +642,13 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -627,10 +668,13 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -650,10 +694,13 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -673,10 +720,13 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -696,10 +746,13 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -719,10 +772,13 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -742,10 +798,13 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -765,10 +824,13 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -788,10 +850,13 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -811,10 +876,13 @@
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -834,10 +902,13 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -857,10 +928,13 @@
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -880,10 +954,13 @@
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -903,10 +980,13 @@
         <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -926,10 +1006,13 @@
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -949,10 +1032,13 @@
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -972,10 +1058,13 @@
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -995,10 +1084,13 @@
         <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1018,10 +1110,13 @@
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1041,10 +1136,13 @@
         <v>25</v>
       </c>
       <c r="G26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1064,10 +1162,13 @@
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1087,10 +1188,13 @@
         <v>27</v>
       </c>
       <c r="G28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1110,6 +1214,9 @@
         <v>28</v>
       </c>
       <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>